<commit_message>
alteração no diretório do arquivo excel
</commit_message>
<xml_diff>
--- a/lista de mercado.xlsx
+++ b/lista de mercado.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>12,75</t>
+          <t>12,70</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -451,12 +451,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Not Milk Chocolate Leite Vegetal 1l</t>
+          <t>Not Milk Chocolate Leite Vegetal 1 Litro</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://produto.mercadolivre.com.br/MLB-1928006924-not-milk-chocolate-leite-vegetal-1l-_JM#position=16&amp;search_layout=grid&amp;type=item&amp;tracking_id=3efc60dc-cc17-4861-894c-2c1841d55818</t>
+          <t>https://produto.mercadolivre.com.br/MLB-2075420500-not-milk-chocolate-leite-vegetal-1-litro-_JM#position=15&amp;search_layout=grid&amp;type=item&amp;tracking_id=0a201942-c81a-4a02-a565-ad4fb8fe7a5f</t>
         </is>
       </c>
     </row>
@@ -478,7 +478,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://produto.mercadolivre.com.br/MLB-2160686438-motorola-moto-e7-32-gb-cinza-metalico-2-gb-ram-_JM?searchVariation=174147059913#searchVariation=174147059913&amp;position=9&amp;search_layout=stack&amp;type=item&amp;tracking_id=70986d21-10f4-478d-97f1-34cf34fb0532</t>
+          <t>https://produto.mercadolivre.com.br/MLB-2160686438-motorola-moto-e7-32-gb-cinza-metalico-2-gb-ram-_JM?searchVariation=174147059913#searchVariation=174147059913&amp;position=9&amp;search_layout=stack&amp;type=item&amp;tracking_id=aa097c06-1ba3-44dd-80f2-935c3436b0a0</t>
         </is>
       </c>
     </row>
@@ -500,7 +500,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/alimento-whiskas-castrados-1-para-gato-adulto-sabor-peixe-em-sach-de-85g/p/MLB18378323?pdp_filters=deal:MLB2407#searchVariation=MLB18378323&amp;position=1&amp;search_layout=grid&amp;type=product&amp;tracking_id=9567b8e3-9e98-425a-9f08-50169af1f196</t>
+          <t>https://www.mercadolivre.com.br/alimento-whiskas-castrados-1-para-gato-adulto-sabor-peixe-em-sach-de-85g/p/MLB18378323?pdp_filters=deal:MLB2407#searchVariation=MLB18378323&amp;position=1&amp;search_layout=grid&amp;type=product&amp;tracking_id=91be6bdd-6492-4e0c-9b50-d5fd5cedec5e</t>
         </is>
       </c>
     </row>
@@ -512,17 +512,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3,39</t>
+          <t>2,98</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Refrigerante Coca-cola Zero 350ml Unid - Original</t>
+          <t>Refrigerante Coca-cola Zero 220ml Unid - Original</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://produto.mercadolivre.com.br/MLB-1850869619-refrigerante-coca-cola-zero-350ml-unid-original-_JM#position=3&amp;search_layout=grid&amp;type=item&amp;tracking_id=59dfdcf3-c88b-40d4-8d16-d896b599b296</t>
+          <t>https://produto.mercadolivre.com.br/MLB-2108100186-refrigerante-coca-cola-zero-220ml-unid-original-_JM#position=1&amp;search_layout=grid&amp;type=item&amp;tracking_id=842d2c8d-462d-4455-86b0-2eb6718ec4a8</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Pequenas organizações e correção preço nagumo
</commit_message>
<xml_diff>
--- a/lista de mercado.xlsx
+++ b/lista de mercado.xlsx
@@ -45,7 +45,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -397,28 +398,28 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col width="24.5703125" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
-    <col width="6.5703125" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-    <col width="6.5703125" customWidth="1" style="2" min="3" max="3"/>
-    <col width="70.7109375" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
-    <col width="255.7109375" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
-    <col width="25.85546875" customWidth="1" style="2" min="6" max="7"/>
-    <col width="80.85546875" bestFit="1" customWidth="1" style="2" min="8" max="8"/>
-    <col width="25.85546875" customWidth="1" style="2" min="9" max="9"/>
+    <col width="24.5703125" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
+    <col width="6.5703125" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
+    <col width="9.28515625" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
+    <col width="70.7109375" bestFit="1" customWidth="1" style="3" min="4" max="4"/>
+    <col width="255.7109375" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
+    <col width="25.85546875" customWidth="1" style="3" min="6" max="7"/>
+    <col width="80.85546875" bestFit="1" customWidth="1" style="3" min="8" max="8"/>
+    <col width="25.85546875" customWidth="1" style="3" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Dados Mercado Livre</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Dados Nagumo</t>
         </is>
@@ -479,22 +480,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>12,70</t>
+          <t>11,19</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>24% OFF</t>
+          <t>34% OFF</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Not Milk Chocolate Leite Vegetal 1 Litro</t>
+          <t>Not Milk Chocolate Leite Vegetal 1l</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://produto.mercadolivre.com.br/MLB-2075420500-not-milk-chocolate-leite-vegetal-1-litro-_JM#position=14&amp;search_layout=grid&amp;type=item&amp;tracking_id=269dab71-1db4-4e8f-8659-38c689c36fe7</t>
+          <t>https://produto.mercadolivre.com.br/MLB-1928006924-not-milk-chocolate-leite-vegetal-1l-_JM#position=13&amp;search_layout=grid&amp;type=item&amp;tracking_id=81ee5baf-aeab-4203-83b1-9afa27befcbb</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -516,22 +517,47 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Motorola E7</t>
+          <t>Molho de Tomate Bolonhesa Heinz 340G</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>629,90</t>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>---</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Motorola Moto E7 32 Gb Cinza-metálico 2 Gb Ram</t>
+          <t>Produto não encontrado</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://produto.mercadolivre.com.br/MLB-2160686438-motorola-moto-e7-32-gb-cinza-metalico-2-gb-ram-_JM?searchVariation=174147059913#searchVariation=174147059913&amp;position=9&amp;search_layout=stack&amp;type=item&amp;tracking_id=21b0426f-e4fa-4675-9926-e4cd565121f8</t>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">R$ 5,08 </t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Heinz L4P3 </t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Molho de Tomate Bolonhesa Heinz 340G</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>http://www.nagumo.com.br/atibaia-lj32-atibaia-alvinopolis-avenida-prof-carlos-alberto-de-carvalho/produto/molho-de-tomate-bolonhesa-heinz-340g</t>
         </is>
       </c>
     </row>
@@ -543,22 +569,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2,59</t>
+          <t>2,44</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>---</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Alimento Whiskas Castrados 1+ para gato adulto sabor peixe em sachê de 85g</t>
+          <t>Whiskas Sachê Peixe Ao Molho Gatos Castrados 85g</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://www.mercadolivre.com.br/alimento-whiskas-castrados-1-para-gato-adulto-sabor-peixe-em-sach-de-85g/p/MLB18378323?pdp_filters=deal:MLB2407#searchVariation=MLB18378323&amp;position=1&amp;search_layout=grid&amp;type=product&amp;tracking_id=c1a9a3c6-2f25-41fa-ae58-0abd42d4eb13</t>
+          <t>https://produto.mercadolivre.com.br/MLB-1887314682-whiskas-sach-peixe-ao-molho-gatos-castrados-85g-_JM#position=6&amp;search_layout=grid&amp;type=item&amp;tracking_id=098de6a2-70a8-4b14-93a3-77972dd860ac</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t xml:space="preserve">R$ 3,16 </t>
+          <t>R$ 3,16</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Poupe R$ 0,67</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -580,37 +616,37 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2,28</t>
+          <t>1,29</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>18% OFF</t>
+          <t>21% OFF</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Refrigerante Coca-cola Zero 220ml Unid - Original</t>
+          <t>Refrigerante Coca-Cola Sem Açúcar Pet 200ml</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://produto.mercadolivre.com.br/MLB-2108779670-refrigerante-coca-cola-zero-220ml-unid-original-_JM#position=1&amp;search_layout=grid&amp;type=item&amp;tracking_id=c50dbc50-251b-41ea-b8d8-11ab00a238f0</t>
+          <t>https://www.mercadolivre.com.br/refrigerante-coca-cola-sem-acucar-pet-200ml/p/MLB18306379?pdp_filters=deal:MLB2407#searchVariation=MLB18306379&amp;position=1&amp;search_layout=grid&amp;type=product&amp;tracking_id=1e2ed2cf-88ee-453c-8a3a-f443b0f141db</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t xml:space="preserve">R$ 4,55 </t>
+          <t xml:space="preserve">R$ 10,17 </t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Coca-Cola sem Açúcar 600Ml</t>
+          <t>Coca-Cola sem Açúcar 2,5L</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>http://www.nagumo.com.br/atibaia-lj32-atibaia-alvinopolis-avenida-prof-carlos-alberto-de-carvalho/produto/coca-cola-sem-acucar-600ml</t>
+          <t>http://www.nagumo.com.br/atibaia-lj32-atibaia-alvinopolis-avenida-prof-carlos-alberto-de-carvalho/produto/coca-cola-sem-acucar-2-5l</t>
         </is>
       </c>
     </row>
@@ -618,6 +654,26 @@
       <c r="A7" t="inlineStr">
         <is>
           <t>tira manchas gel multiuso vanish sachê 500ml</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Produto não encontrado</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>---</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">

</xml_diff>